<commit_message>
added exercises to section 6
</commit_message>
<xml_diff>
--- a/output/dados_pesquisa_fake_news.xlsx
+++ b/output/dados_pesquisa_fake_news.xlsx
@@ -546,12 +546,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jonathan</t>
+          <t>Ysadora</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -566,49 +566,49 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Não binário</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Agnóstico</t>
+          <t>Espírita</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Centro Esquerda</t>
+          <t>Extrema Direita</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Prefiro não dizer</t>
+          <t>Divorciado</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Com pais ou responsáveis</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>&lt;1</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>7018</v>
+        <v>5557</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Relações Públicas</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Moderada</t>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -632,12 +632,12 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Televisão e/ou Rádio</t>
+          <t>Redes Sociais</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>Compartilhando por familiares e amigos</t>
+          <t>As pessoas acreditam em notícias que lhes convêm</t>
         </is>
       </c>
     </row>
@@ -647,17 +647,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Francielly</t>
+          <t>Talita</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>25-34</t>
+          <t>35-44</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -672,22 +672,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Católica</t>
+          <t>Agnóstico</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Extrema Direita</t>
+          <t>Centro Direita</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Viúvo</t>
+          <t>Casado</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -697,11 +697,11 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>&gt;10</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>8329</v>
+        <v>6054</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -709,36 +709,36 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Sim, porém pouco</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Baixa</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
           <t>Moderada</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Baixa</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Moderada</t>
-        </is>
-      </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Portais de notícias</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>Desinformação</t>
+          <t>Compartilhando por familiares e amigos</t>
         </is>
       </c>
     </row>
@@ -748,7 +748,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Amanda</t>
+          <t>Jonathan</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -758,88 +758,88 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>35-44</t>
+          <t>45-54</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>Outro</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Não binário</t>
-        </is>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Agnóstico</t>
+          <t>Espírita</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Esquerda</t>
+          <t>Direita</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Divorciado</t>
+          <t>Casado</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Com amigos</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>&gt;10</t>
+          <t>7-10</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>5256</v>
+        <v>9547</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Relações Públicas</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Não sei</t>
+          <t>Sim, porém pouco</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
+          <t>Moderada</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
           <t>Baixa</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Alta</t>
+          <t>Moderada</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>E-mail</t>
+          <t>Portais de notícias</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>Ausência das agências de checagem</t>
+          <t>Confiança excessiva em fontes duvidosas</t>
         </is>
       </c>
     </row>
@@ -849,65 +849,65 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Maria</t>
+          <t>Marcos</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>&lt;18</t>
+          <t>55-64</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Prefiro não dizer</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Prefiro não dizer</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Espírita</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Centro</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Viúvo</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
           <t>Outro</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Prefiro não dizer</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Evangélica</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Extrema Esquerda</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Divorciado</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Sozinho</t>
-        </is>
-      </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>7-10</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>9612</v>
+        <v>7777</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Cinema e Audiovisual</t>
         </is>
       </c>
       <c r="O5" t="n">
@@ -915,19 +915,19 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Não sei</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
+          <t>Moderada</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
           <t>Baixa</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
       <c r="S5" t="inlineStr">
         <is>
           <t>Baixa</t>
@@ -935,12 +935,12 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>E-mail</t>
+          <t>Portais de notícias</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>Quando a manchete chama muita atenção</t>
+          <t>A forma como a notícia é apresentada</t>
         </is>
       </c>
     </row>
@@ -950,7 +950,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>Francielly</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -960,7 +960,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>&lt;18</t>
+          <t>35-44</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -970,22 +970,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>Transgênero</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>Prefiro não dizer</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Prefiro não dizer</t>
-        </is>
-      </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Católica</t>
+          <t>Espírita</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Extrema Direita</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1000,19 +1000,19 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>&gt;10</t>
+          <t>7-10</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>6105</v>
+        <v>5316</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Relações Públicas</t>
+          <t>Jornalismo</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Baixa</t>
+          <t>Moderada</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1036,12 +1036,12 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>E-mail</t>
+          <t>Televisão e/ou Rádio</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>Desinformação</t>
+          <t>Confiança excessiva em fontes duvidosas</t>
         </is>
       </c>
     </row>
@@ -1051,17 +1051,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ysadora</t>
+          <t>Vanessa</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>35-44</t>
+          <t>18-24</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1071,12 +1071,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Prefiro não dizer</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1086,30 +1086,30 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Extrema Esquerda</t>
+          <t>Extrema Direita</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Prefiro não dizer</t>
+          <t>Solteiro</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Sozinho</t>
+          <t>Com parceiro e/ou filhos</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>&lt;1</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>7463</v>
+        <v>9595</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Relações Públicas</t>
         </is>
       </c>
       <c r="O7" t="n">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Sim, muito diferentes</t>
+          <t>Não são diferentes</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1132,17 +1132,17 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Alta</t>
+          <t>Moderada</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>Redes Sociais</t>
+          <t>E-mail</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>Compartilhamento por influenciadores</t>
+          <t>Outro</t>
         </is>
       </c>
     </row>
@@ -1152,27 +1152,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rayane</t>
+          <t>Ysadora</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>25-34</t>
+          <t>55-64</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Transgênero</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Esquerda</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1197,16 +1197,16 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sozinho</t>
+          <t>Com amigos</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>7123</v>
+        <v>7232</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1214,7 +1214,7 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -1223,27 +1223,27 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Alta</t>
+          <t>Moderada</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
+          <t>Baixa</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
           <t>Moderada</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>Moderada</t>
-        </is>
-      </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>E-mail</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>Ausência das agências de checagem</t>
+          <t>Quando a manchete chama muita atenção</t>
         </is>
       </c>
     </row>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1263,51 +1263,51 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>65+</t>
+          <t>&lt;18</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Prefiro não dizer</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Ateu</t>
+          <t>Evangélica</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Centro Direita</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Prefiro não dizer</t>
+          <t>Casado</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Com amigos</t>
+          <t>Com parceiro e/ou filhos</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>&lt;1</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>5748</v>
+        <v>6684</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1329,22 +1329,22 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>Moderada</t>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Baixa</t>
+          <t>Alta</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Redes Sociais</t>
+          <t>E-mail</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>Compartilhando por familiares e amigos</t>
+          <t>As pessoas acreditam em notícias que lhes convêm</t>
         </is>
       </c>
     </row>
@@ -1354,37 +1354,37 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>Ysadora</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>&lt;18</t>
+          <t>65+</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Cisgênero</t>
+          <t>Não binário</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Católica</t>
+          <t>Outras</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1399,48 +1399,48 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Com amigos</t>
+          <t>Com pais ou responsáveis</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>&gt;10</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>8131</v>
+        <v>6980</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Jornalismo</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Não sei</t>
+          <t>Sim, porém pouco</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
           <t>Baixa</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>Moderada</t>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>Portais de notícias</t>
+          <t>Televisão e/ou Rádio</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -1455,98 +1455,98 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Jonathan</t>
+          <t>Thiago</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>25-34</t>
+          <t>65+</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Transgênero</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Parda</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Espírita</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Direita</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Viúvo</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Sozinho</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>1-3</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>8777</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Cinema e Audiovisual</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>7</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Não são diferentes</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>E-mail</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
           <t>Outro</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Outro</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Prefiro não dizer</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Outras</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Não se interessa</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Casado</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Com parceiro e/ou filhos</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>4-6</t>
-        </is>
-      </c>
-      <c r="M11" t="n">
-        <v>7714</v>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>Jornalismo</t>
-        </is>
-      </c>
-      <c r="O11" t="n">
-        <v>1</v>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>Sim, muito diferentes</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>Moderada</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>Portais de notícias</t>
-        </is>
-      </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>Quando a manchete chama muita atenção</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added exercises for Section 7
</commit_message>
<xml_diff>
--- a/output/dados_pesquisa_fake_news.xlsx
+++ b/output/dados_pesquisa_fake_news.xlsx
@@ -546,42 +546,42 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ysadora</t>
+          <t>Amanda</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>18-24</t>
+          <t>55-64</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Prefiro não dizer</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Espírita</t>
+          <t>Ateu</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Extrema Direita</t>
+          <t>Centro Direita</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -600,11 +600,11 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>5557</v>
+        <v>9937</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Relações Públicas</t>
+          <t>Cinema e Audiovisual</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -612,24 +612,24 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Não sei</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
+          <t>Moderada</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
           <t>Alta</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>Baixa</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
       <c r="T2" t="inlineStr">
         <is>
           <t>Redes Sociais</t>
@@ -637,7 +637,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>As pessoas acreditam em notícias que lhes convêm</t>
+          <t>Ausência das agências de checagem</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Talita</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -657,88 +657,88 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>35-44</t>
+          <t>65+</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Cisgênero</t>
+          <t>Prefiro não dizer</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Agnóstico</t>
+          <t>Evangélica</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Centro Direita</t>
+          <t>Esquerda</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Casado</t>
+          <t>Viúvo</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Com parceiro e/ou filhos</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>&gt;10</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>6054</v>
+        <v>9994</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Publicidade e Propaganda</t>
+          <t>Relações Públicas</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Não sei</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
+          <t>Baixa</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
           <t>Alta</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Baixa</t>
-        </is>
-      </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Moderada</t>
+          <t>Alta</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Portais de notícias</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>Compartilhando por familiares e amigos</t>
+          <t>A forma como a notícia é apresentada</t>
         </is>
       </c>
     </row>
@@ -748,17 +748,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jonathan</t>
+          <t>Marcos</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>45-54</t>
+          <t>18-24</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -768,12 +768,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Não binário</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -783,38 +783,38 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Direita</t>
+          <t>Não se interessa</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Casado</t>
+          <t>Solteiro</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Sozinho</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>7-10</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>9547</v>
+        <v>8271</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Relações Públicas</t>
+          <t>Cinema e Audiovisual</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Sim, porém pouco</t>
+          <t>Não sei</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Baixa</t>
+          <t>Moderada</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -834,12 +834,12 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Portais de notícias</t>
+          <t>Televisão e/ou Rádio</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>Confiança excessiva em fontes duvidosas</t>
+          <t>A forma como a notícia é apresentada</t>
         </is>
       </c>
     </row>
@@ -849,17 +849,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Marcos</t>
+          <t>Thiago</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>55-64</t>
+          <t>25-34</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -869,27 +869,27 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Prefiro não dizer</t>
+          <t>Não binário</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Prefiro não dizer</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Espírita</t>
+          <t>Católica</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Centro Esquerda</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Viúvo</t>
+          <t>Divorciado</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -899,40 +899,40 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>7-10</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>7777</v>
+        <v>8143</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Cinema e Audiovisual</t>
+          <t>Publicidade e Propaganda</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Não sei</t>
+          <t>Não</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Moderada</t>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
           <t>Baixa</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>Baixa</t>
-        </is>
-      </c>
       <c r="T5" t="inlineStr">
         <is>
           <t>Portais de notícias</t>
@@ -940,7 +940,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>A forma como a notícia é apresentada</t>
+          <t>Outro</t>
         </is>
       </c>
     </row>
@@ -950,42 +950,42 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Francielly</t>
+          <t>Rayane</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>35-44</t>
+          <t>65+</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>Outro</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Transgênero</t>
-        </is>
-      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Prefiro não dizer</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Espírita</t>
+          <t>Outras</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Extrema Direita</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -995,53 +995,53 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Com parceiro e/ou filhos</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>7-10</t>
+          <t>&lt;1</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>5316</v>
+        <v>6765</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Jornalismo</t>
+          <t>Cinema e Audiovisual</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Não sei</t>
+          <t>Sim, muito diferentes</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
           <t>Moderada</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>Televisão e/ou Rádio</t>
+          <t>Redes Sociais</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>Confiança excessiva em fontes duvidosas</t>
+          <t>As pessoas acreditam em notícias que lhes convêm</t>
         </is>
       </c>
     </row>
@@ -1051,17 +1051,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Vanessa</t>
+          <t>Ysadora</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>18-24</t>
+          <t>25-34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1076,22 +1076,22 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Ateu</t>
+          <t>Agnóstico</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Extrema Direita</t>
+          <t>Não se interessa</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Solteiro</t>
+          <t>Casado</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1101,48 +1101,48 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>&lt;1</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>9595</v>
+        <v>6267</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Relações Públicas</t>
+          <t>Publicidade e Propaganda</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Não são diferentes</t>
+          <t>Sim, muito diferentes</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Baixa</t>
+          <t>Alta</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>Baixa</t>
+          <t>Moderada</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Moderada</t>
+          <t>Alta</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>E-mail</t>
+          <t>Aplicativos de mensagem</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Polarização</t>
         </is>
       </c>
     </row>
@@ -1152,98 +1152,98 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ysadora</t>
+          <t>Jonathan</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>55-64</t>
+          <t>&lt;18</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Não binário</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Prefiro não dizer</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Evangélica</t>
+          <t>Católica</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Esquerda</t>
+          <t>Direita</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Prefiro não dizer</t>
+          <t>Divorciado</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Com amigos</t>
+          <t>Sozinho</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>&lt;1</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>7232</v>
+        <v>7462</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Relações Públicas</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Sim, porém pouco</t>
+          <t>Não sei</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
+          <t>Baixa</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
           <t>Moderada</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>Baixa</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>Moderada</t>
-        </is>
-      </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Aplicativos de mensagem</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>Quando a manchete chama muita atenção</t>
+          <t>Compartilhamento por influenciadores</t>
         </is>
       </c>
     </row>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>Talita</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1263,51 +1263,51 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>&lt;18</t>
+          <t>35-44</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Prefiro não dizer</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Evangélica</t>
+          <t>Outras</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Centro Direita</t>
+          <t>Extrema Esquerda</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Casado</t>
+          <t>Divorciado</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Com parceiro e/ou filhos</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>6684</v>
+        <v>5481</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1315,36 +1315,36 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Sim, muito diferentes</t>
+          <t>Sim, porém pouco</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
           <t>Baixa</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>Baixa</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>E-mail</t>
+          <t>Redes Sociais</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>As pessoas acreditam em notícias que lhes convêm</t>
+          <t>Polarização</t>
         </is>
       </c>
     </row>
@@ -1354,22 +1354,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ysadora</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>65+</t>
+          <t>18-24</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1379,27 +1379,27 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Outras</t>
+          <t>Judaíca</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Direita</t>
+          <t>Centro Direita</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Viúvo</t>
+          <t>Prefiro não dizer</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Com pais ou responsáveis</t>
+          <t>Com parceiro e/ou filhos</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1408,34 +1408,34 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>6980</v>
+        <v>5050</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Jornalismo</t>
+          <t>Cinema e Audiovisual</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Sim, porém pouco</t>
+          <t>Não são diferentes</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
+          <t>Baixa</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
           <t>Alta</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Baixa</t>
-        </is>
-      </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>Baixa</t>
+          <t>Alta</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>Quando a manchete chama muita atenção</t>
+          <t>Compartilhamento por influenciadores</t>
         </is>
       </c>
     </row>
@@ -1455,17 +1455,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>65+</t>
+          <t>45-54</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1480,68 +1480,68 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Espírita</t>
+          <t>Ateu</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Direita</t>
+          <t>Extrema Esquerda</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Viúvo</t>
+          <t>Divorciado</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Sozinho</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>&gt;10</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>8777</v>
+        <v>7461</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Cinema e Audiovisual</t>
+          <t>Relações Públicas</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Não são diferentes</t>
+          <t>Sim, porém pouco</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Alta</t>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>Alta</t>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>Alta</t>
+          <t>Baixa</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>E-mail</t>
+          <t>Aplicativos de mensagem</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">

</xml_diff>